<commit_message>
updated grading rubric still can't figure out the menu screen
</commit_message>
<xml_diff>
--- a/Rubric.xlsx
+++ b/Rubric.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="30">
   <si>
     <t>The Game</t>
   </si>
@@ -88,6 +88,24 @@
   </si>
   <si>
     <t>executable file name and icon</t>
+  </si>
+  <si>
+    <t>in progress</t>
+  </si>
+  <si>
+    <t>done</t>
+  </si>
+  <si>
+    <t>20 enemies … porbably done</t>
+  </si>
+  <si>
+    <t>possibly done I just changed the colors of the stars we could do different images though</t>
+  </si>
+  <si>
+    <t xml:space="preserve">same as MP3 </t>
+  </si>
+  <si>
+    <t>150 enemies - done</t>
   </si>
 </sst>
 </file>
@@ -438,86 +456,107 @@
   <dimension ref="A1:B26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="41.5546875" customWidth="1"/>
-    <col min="2" max="2" width="37.77734375" customWidth="1"/>
+    <col min="2" max="2" width="48.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B9" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B10" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B11" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B12" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B14" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>16</v>
       </c>

</xml_diff>